<commit_message>
Done. Time for refactor
</commit_message>
<xml_diff>
--- a/zad4/Sprawozdanie/data.xlsx
+++ b/zad4/Sprawozdanie/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>rozmiar</t>
   </si>
@@ -60,9 +60,6 @@
     <t>WZORY</t>
   </si>
   <si>
-    <t>F(x)=-0.000609+0.00000108x</t>
-  </si>
-  <si>
     <t>F(x)=0,2387823693205711 -0,0008012150098502  x+0,0000003535496443 x^2+0,0000000002725663 x^3</t>
   </si>
   <si>
@@ -72,7 +69,28 @@
     <t>F(x)=1,9597370696668281-0,0053390356114687x+0,0000027282285294  x^2</t>
   </si>
   <si>
-    <t>F(x)=-0,0178824102691862+0,0000207193142874*D142</t>
+    <t>F(x)=-0,0003470911688645 +0,0000007125249395x</t>
+  </si>
+  <si>
+    <t>F(x)=-0,0316993039054592+0,0000491746627289*D142</t>
+  </si>
+  <si>
+    <t>23.9645</t>
+  </si>
+  <si>
+    <t>0.132</t>
+  </si>
+  <si>
+    <t>62.916499999999999</t>
+  </si>
+  <si>
+    <t>1046.851</t>
+  </si>
+  <si>
+    <t>96.89</t>
+  </si>
+  <si>
+    <t>0.171</t>
   </si>
 </sst>
 </file>
@@ -82,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,14 +145,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -230,17 +240,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -298,7 +309,7 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -324,9 +335,9 @@
     <xf numFmtId="164" fontId="5" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="12"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="13"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="12"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="14"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -337,12 +348,12 @@
     <cellStyle name="20% - Accent6" xfId="11" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="14" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="8" builtinId="43"/>
-    <cellStyle name="Accent2" xfId="14" builtinId="33"/>
-    <cellStyle name="Bad" xfId="12" builtinId="27"/>
+    <cellStyle name="Accent2" xfId="13" builtinId="33"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="13" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="12" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -995,11 +1006,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="119716096"/>
-        <c:axId val="120463360"/>
+        <c:axId val="115460352"/>
+        <c:axId val="116076544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119716096"/>
+        <c:axId val="115460352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,14 +1027,14 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120463360"/>
-        <c:crossesAt val="5.0000000000000106E-6"/>
+        <c:crossAx val="116076544"/>
+        <c:crossesAt val="5.0000000000000123E-6"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120463360"/>
+        <c:axId val="116076544"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1032,7 +1043,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119716096"/>
+        <c:crossAx val="115460352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1045,7 +1056,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1062,9 +1073,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="7.5770125235833582E-2"/>
-          <c:y val="8.9314548085144538E-2"/>
+          <c:y val="8.9314548085144552E-2"/>
           <c:w val="0.78450675362118283"/>
-          <c:h val="0.8023122298896016"/>
+          <c:h val="0.80231222988960138"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1879,76 +1890,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1.9000000000000001E-5</c:v>
+                  <c:v>1.2990000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1999999999999997E-5</c:v>
+                  <c:v>3.6000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3200000000000001E-4</c:v>
+                  <c:v>7.7990000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1000000000000001E-4</c:v>
+                  <c:v>1.449E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.39E-4</c:v>
+                  <c:v>2.7299999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.7600000000000001E-4</c:v>
+                  <c:v>4.0099999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2799999999999996E-4</c:v>
+                  <c:v>6.1190000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2329999999999999E-3</c:v>
+                  <c:v>8.8000000000000005E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7600000000000001E-3</c:v>
+                  <c:v>1.157E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.398E-3</c:v>
+                  <c:v>1.4069999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0469999999999998E-3</c:v>
+                  <c:v>2.0889999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1809999999999998E-3</c:v>
+                  <c:v>2.7130000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9280000000000001E-3</c:v>
+                  <c:v>3.5400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.1579999999999995E-3</c:v>
+                  <c:v>4.9849999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.273E-2</c:v>
+                  <c:v>6.1679999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8724999999999999E-2</c:v>
+                  <c:v>7.5380000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.7199999999999998E-2</c:v>
+                  <c:v>9.3100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5430000000000003E-2</c:v>
+                  <c:v>0.116274</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.4810000000000003E-2</c:v>
+                  <c:v>0.13095000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.8700000000000002E-2</c:v>
+                  <c:v>0.15928</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3520000000000002E-2</c:v>
+                  <c:v>0.18890000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.8429999999999995E-2</c:v>
+                  <c:v>0.21460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11020000000000001</c:v>
+                  <c:v>0.25740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.12706999999999999</c:v>
+                  <c:v>0.26429999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2053,90 +2064,90 @@
             <c:numRef>
               <c:f>Sheet1!$K$63:$K$86</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>1.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1E-5</c:v>
+                  <c:v>2.0000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9000000000000001E-5</c:v>
+                  <c:v>3.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8999999999999999E-5</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2000000000000002E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4200000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.42E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0699999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.17E-4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.8399999999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.3100000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0709999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.2949999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.5900000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.882E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.4220000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.7520000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.176E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.692E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.2249999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.6100000000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.1900000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.7800000000000004E-3</c:v>
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1.2899999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.7899999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.1900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.5900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>2.7999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.6900000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>5.1900000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>7.7899999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1.0189999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.16E-3</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1.4189999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>1.7390000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>1.8500000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>2.1900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>2.7399999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>3.15E-3</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>3.4499999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>3.8500000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="120505088"/>
-        <c:axId val="120506624"/>
+        <c:axId val="116126464"/>
+        <c:axId val="116128000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120505088"/>
+        <c:axId val="116126464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2153,14 +2164,14 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120506624"/>
-        <c:crossesAt val="1.0000000000000016E-6"/>
+        <c:crossAx val="116128000"/>
+        <c:crossesAt val="1.0000000000000021E-6"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120506624"/>
+        <c:axId val="116128000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2179,7 +2190,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120505088"/>
+        <c:crossAx val="116126464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2190,10 +2201,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.85744660960538621"/>
-          <c:y val="2.2164938557743173E-2"/>
-          <c:w val="0.13926865896149601"/>
-          <c:h val="0.66679988900078091"/>
+          <c:x val="0.85744660960538632"/>
+          <c:y val="2.216493855774318E-2"/>
+          <c:w val="0.13926865896149604"/>
+          <c:h val="0.66679988900078113"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2211,7 +2222,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2229,7 +2240,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12214520059992502"/>
-          <c:y val="2.9221892150779517E-2"/>
+          <c:y val="2.9221892150779527E-2"/>
           <c:w val="0.82982658417697786"/>
           <c:h val="0.94155621569844095"/>
         </c:manualLayout>
@@ -2330,76 +2341,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-1.61419878690446E-2</c:v>
+                  <c:v>-2.7568632236231599E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.4898829011800599E-2</c:v>
+                  <c:v>-2.4618152472497601E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.33241611259582E-2</c:v>
+                  <c:v>-2.0880878105101197E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.14179842115174E-2</c:v>
+                  <c:v>-1.6356809134042399E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-9.1802982684781997E-3</c:v>
+                  <c:v>-1.1045945559321198E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-6.6111032968405991E-3</c:v>
+                  <c:v>-4.9482873809376E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.7103992966045999E-3</c:v>
+                  <c:v>1.9361654011084001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.7818626777020035E-4</c:v>
+                  <c:v>9.6074127868168019E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0855357896625996E-3</c:v>
+                  <c:v>1.8065454776187602E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9807668756937981E-3</c:v>
+                  <c:v>2.73102913692208E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1207506990323399E-2</c:v>
+                  <c:v>3.7341922565916404E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5765756133551401E-2</c:v>
+                  <c:v>4.8160348366274398E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0655514305377796E-2</c:v>
+                  <c:v>5.9765568770294798E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5876781505802599E-2</c:v>
+                  <c:v>7.2157583777977596E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1429557734825794E-2</c:v>
+                  <c:v>8.5336393389322807E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7313842992447402E-2</c:v>
+                  <c:v>9.9301997604330394E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.3529637278667391E-2</c:v>
+                  <c:v>0.11405439642300041</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.0076940593485789E-2</c:v>
+                  <c:v>0.12959358984533281</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.6955752936902596E-2</c:v>
+                  <c:v>0.14591957787132759</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.4166074308917798E-2</c:v>
+                  <c:v>0.1630323605009848</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.1707904709531395E-2</c:v>
+                  <c:v>0.18093193773430441</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.9581244138743387E-2</c:v>
+                  <c:v>0.1996183095712864</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.7786092596553789E-2</c:v>
+                  <c:v>0.21909147601193077</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.6322450082962585E-2</c:v>
+                  <c:v>0.2393514370562376</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2508,99 +2519,99 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1.9000000000000001E-5</c:v>
+                  <c:v>1.2990000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1999999999999997E-5</c:v>
+                  <c:v>3.6000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3200000000000001E-4</c:v>
+                  <c:v>7.7990000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1000000000000001E-4</c:v>
+                  <c:v>1.449E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.39E-4</c:v>
+                  <c:v>2.7299999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.7600000000000001E-4</c:v>
+                  <c:v>4.0099999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2799999999999996E-4</c:v>
+                  <c:v>6.1190000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2329999999999999E-3</c:v>
+                  <c:v>8.8000000000000005E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7600000000000001E-3</c:v>
+                  <c:v>1.157E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.398E-3</c:v>
+                  <c:v>1.4069999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0469999999999998E-3</c:v>
+                  <c:v>2.0889999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1809999999999998E-3</c:v>
+                  <c:v>2.7130000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9280000000000001E-3</c:v>
+                  <c:v>3.5400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.1579999999999995E-3</c:v>
+                  <c:v>4.9849999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.273E-2</c:v>
+                  <c:v>6.1679999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.8724999999999999E-2</c:v>
+                  <c:v>7.5380000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.7199999999999998E-2</c:v>
+                  <c:v>9.3100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.5430000000000003E-2</c:v>
+                  <c:v>0.116274</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.4810000000000003E-2</c:v>
+                  <c:v>0.13095000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.8700000000000002E-2</c:v>
+                  <c:v>0.15928</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3520000000000002E-2</c:v>
+                  <c:v>0.18890000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.8429999999999995E-2</c:v>
+                  <c:v>0.21460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11020000000000001</c:v>
+                  <c:v>0.25740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.12706999999999999</c:v>
+                  <c:v>0.26429999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="120467456"/>
-        <c:axId val="120538624"/>
+        <c:axId val="116084736"/>
+        <c:axId val="116151808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120467456"/>
+        <c:axId val="116084736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120538624"/>
-        <c:crossesAt val="1.0000000000000004E-5"/>
+        <c:crossAx val="116151808"/>
+        <c:crossesAt val="1.0000000000000008E-5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120538624"/>
+        <c:axId val="116151808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,7 +2619,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120467456"/>
+        <c:crossAx val="116084736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2628,7 +2639,7 @@
           <c:x val="0.1612907761529809"/>
           <c:y val="3.6548814996545234E-2"/>
           <c:w val="0.30403595925161198"/>
-          <c:h val="0.20970741632813278"/>
+          <c:h val="0.20970741632813281"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2646,7 +2657,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2696,8 +2707,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23694344959266564"/>
-          <c:y val="2.6264327500860312E-2"/>
+          <c:x val="0.23694344959266572"/>
+          <c:y val="2.6264327500860316E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2709,9 +2720,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.9647240900718045E-2"/>
-          <c:y val="0.18635781196230511"/>
-          <c:w val="0.86227971761257527"/>
-          <c:h val="0.79577065741059372"/>
+          <c:y val="0.18635781196230514"/>
+          <c:w val="0.8622797176125756"/>
+          <c:h val="0.79577065741059394"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2906,6 +2917,13 @@
                 <a:srgbClr val="92D050"/>
               </a:solidFill>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:spPr>
@@ -2919,6 +2937,13 @@
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="65000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -3085,11 +3110,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="120600064"/>
-        <c:axId val="120601600"/>
+        <c:axId val="116221056"/>
+        <c:axId val="116222976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120600064"/>
+        <c:axId val="116221056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3106,12 +3131,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120601600"/>
+        <c:crossAx val="116222976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120601600"/>
+        <c:axId val="116222976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,7 +3154,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120600064"/>
+        <c:crossAx val="116221056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3141,9 +3166,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.7992334405241193E-2"/>
-          <c:y val="0.17970239001244143"/>
-          <c:w val="0.31310142424012238"/>
-          <c:h val="0.25696480331948013"/>
+          <c:y val="0.17970239001244148"/>
+          <c:w val="0.31310142424012233"/>
+          <c:h val="0.25696480331948029"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3161,7 +3186,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3208,8 +3233,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23993660112636164"/>
-          <c:y val="2.0985535265407123E-2"/>
+          <c:x val="0.2399366011263617"/>
+          <c:y val="2.098553526540713E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3220,9 +3245,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13788647596084794"/>
-          <c:y val="0.16829159979592806"/>
-          <c:w val="0.81385721315837189"/>
+          <c:x val="0.13788647596084791"/>
+          <c:y val="0.16829159979592809"/>
+          <c:w val="0.81385721315837212"/>
           <c:h val="0.80244597154146602"/>
         </c:manualLayout>
       </c:layout>
@@ -3322,76 +3347,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-5.1827999999999998E-4</c:v>
+                  <c:v>-2.8723907394650002E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.5347999999999992E-4</c:v>
+                  <c:v>-2.4448757757650002E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.7139999999999992E-4</c:v>
+                  <c:v>-1.9033568217450002E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.7203999999999992E-4</c:v>
+                  <c:v>-1.2478338774050003E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.5539999999999993E-4</c:v>
+                  <c:v>-4.783069427450004E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.1479999999999937E-5</c:v>
+                  <c:v>4.0522398223499941E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2972000000000005E-4</c:v>
+                  <c:v>1.4027588975349997E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9820000000000009E-4</c:v>
+                  <c:v>2.5142978031549994E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8396000000000008E-4</c:v>
+                  <c:v>3.7398406990949996E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.8700000000000011E-4</c:v>
+                  <c:v>5.0793875853549992E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0732000000000009E-4</c:v>
+                  <c:v>6.5329384619349992E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.14492E-3</c:v>
+                  <c:v>8.1004933288350003E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3998000000000003E-3</c:v>
+                  <c:v>9.7820521860550002E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6719600000000003E-3</c:v>
+                  <c:v>1.1577615033594999E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9614000000000003E-3</c:v>
+                  <c:v>1.3487181871454999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2681200000000002E-3</c:v>
+                  <c:v>1.5510752699635E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5921199999999998E-3</c:v>
+                  <c:v>1.7648327518134999E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9334000000000001E-3</c:v>
+                  <c:v>1.9899906326954998E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.29196E-3</c:v>
+                  <c:v>2.2265489126094998E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.6677999999999997E-3</c:v>
+                  <c:v>2.4745075915554998E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.06092E-3</c:v>
+                  <c:v>2.7338666695335E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.47132E-3</c:v>
+                  <c:v>3.0046261465434998E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.8989999999999997E-3</c:v>
+                  <c:v>3.2867860225854998E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.34396E-3</c:v>
+                  <c:v>3.5803462976594998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3529,90 +3554,90 @@
             <c:numRef>
               <c:f>Sheet1!$K$63:$K$86</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>1.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1E-5</c:v>
+                  <c:v>2.0000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9000000000000001E-5</c:v>
+                  <c:v>3.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8999999999999999E-5</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2000000000000002E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4200000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.42E-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0699999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.17E-4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.8399999999999999E-4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.3100000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0709999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.2949999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.5900000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.882E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.4220000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.7520000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.176E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.692E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.2249999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.6100000000000004E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.1900000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.7800000000000004E-3</c:v>
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1.2899999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.7899999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.1900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.5900000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>2.7999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>3.6900000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>5.1900000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>7.7899999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>1.0189999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>1.16E-3</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>1.4189999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>1.7390000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>1.8500000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>2.1900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>2.7399999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>3.15E-3</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>3.4499999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>3.8500000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="78153984"/>
-        <c:axId val="78152448"/>
+        <c:axId val="116231168"/>
+        <c:axId val="116274304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78153984"/>
+        <c:axId val="116231168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3629,12 +3654,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78152448"/>
+        <c:crossAx val="116274304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78152448"/>
+        <c:axId val="116274304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3652,7 +3677,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78153984"/>
+        <c:crossAx val="116231168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3663,10 +3688,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13447618556362631"/>
-          <c:y val="0.16706489611540393"/>
-          <c:w val="0.50183634210259875"/>
-          <c:h val="0.20999857217805937"/>
+          <c:x val="0.13447618556362634"/>
+          <c:y val="0.16706489611540395"/>
+          <c:w val="0.50183634210259864"/>
+          <c:h val="0.2099985721780594"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3684,7 +3709,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3735,8 +3760,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.21002184310739483"/>
-          <c:y val="1.8406806998727675E-2"/>
+          <c:x val="0.21002184310739488"/>
+          <c:y val="1.8406806998727678E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -3748,9 +3773,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10036842890545028"/>
-          <c:y val="0.15804221142567865"/>
-          <c:w val="0.830259944700252"/>
-          <c:h val="0.81276322613973639"/>
+          <c:y val="0.1580422114256787"/>
+          <c:w val="0.83025994470025188"/>
+          <c:h val="0.81276322613973651"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3947,6 +3972,13 @@
                 </a:srgbClr>
               </a:solidFill>
             </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:spPr>
@@ -3963,6 +3995,13 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="65000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -4129,11 +4168,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="121760384"/>
-        <c:axId val="121758464"/>
+        <c:axId val="116290688"/>
+        <c:axId val="116292608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121760384"/>
+        <c:axId val="116290688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4150,12 +4189,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121758464"/>
+        <c:crossAx val="116292608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121758464"/>
+        <c:axId val="116292608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4173,7 +4212,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121760384"/>
+        <c:crossAx val="116290688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4185,9 +4224,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11064812891187173"/>
-          <c:y val="0.16320025839927033"/>
-          <c:w val="0.32568350337502217"/>
-          <c:h val="0.17398594332815362"/>
+          <c:y val="0.16320025839927035"/>
+          <c:w val="0.33767644736891805"/>
+          <c:h val="0.21079955732560895"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -4205,7 +4244,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4246,15 +4285,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>835400</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>16807</xdr:rowOff>
+      <xdr:colOff>159125</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>35857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1391478</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>33054</xdr:rowOff>
+      <xdr:colOff>1343853</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>52104</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4756,10 +4795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D3:R165"/>
+  <dimension ref="D3:R167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C165" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K168" sqref="K168"/>
+    <sheetView tabSelected="1" topLeftCell="D72" workbookViewId="0">
+      <selection activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5491,7 +5530,11 @@
         <v>19.536000000000001</v>
       </c>
     </row>
-    <row r="61" spans="5:12" ht="15.75" thickBot="1"/>
+    <row r="61" spans="5:12" ht="15.75" thickBot="1">
+      <c r="K61" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
     <row r="62" spans="5:12" ht="16.5" thickTop="1" thickBot="1">
       <c r="E62" t="s">
         <v>6</v>
@@ -5537,11 +5580,11 @@
       <c r="J63" s="6">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="K63" s="7">
-        <v>5.0000000000000004E-6</v>
+      <c r="K63" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="L63" s="13">
-        <v>1.9000000000000001E-5</v>
+        <v>1.2990000000000001E-4</v>
       </c>
     </row>
     <row r="64" spans="5:12">
@@ -5563,11 +5606,11 @@
       <c r="J64" s="6">
         <v>3.16E-3</v>
       </c>
-      <c r="K64" s="7">
-        <v>1.1E-5</v>
+      <c r="K64" s="1">
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="L64" s="13">
-        <v>5.1999999999999997E-5</v>
+        <v>3.6000000000000002E-4</v>
       </c>
     </row>
     <row r="65" spans="5:12">
@@ -5589,11 +5632,11 @@
       <c r="J65" s="6">
         <v>1.0919999999999999E-2</v>
       </c>
-      <c r="K65" s="7">
-        <v>1.9000000000000001E-5</v>
+      <c r="K65" s="1">
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L65" s="13">
-        <v>1.3200000000000001E-4</v>
+        <v>7.7990000000000004E-4</v>
       </c>
     </row>
     <row r="66" spans="5:12">
@@ -5615,11 +5658,11 @@
       <c r="J66" s="6">
         <v>2.0879999999999999E-2</v>
       </c>
-      <c r="K66" s="7">
-        <v>3.8999999999999999E-5</v>
+      <c r="K66" s="1">
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="L66" s="13">
-        <v>2.1000000000000001E-4</v>
+        <v>1.449E-3</v>
       </c>
     </row>
     <row r="67" spans="5:12">
@@ -5641,11 +5684,11 @@
       <c r="J67" s="6">
         <v>3.9259999999999899E-2</v>
       </c>
-      <c r="K67" s="7">
-        <v>7.2000000000000002E-5</v>
+      <c r="K67" s="1">
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="L67" s="13">
-        <v>3.39E-4</v>
+        <v>2.7299999999999998E-3</v>
       </c>
     </row>
     <row r="68" spans="5:12">
@@ -5668,10 +5711,10 @@
         <v>7.7579999999999996E-2</v>
       </c>
       <c r="K68" s="7">
-        <v>1E-4</v>
+        <v>1.2899999999999999E-4</v>
       </c>
       <c r="L68" s="13">
-        <v>5.7600000000000001E-4</v>
+        <v>4.0099999999999997E-3</v>
       </c>
     </row>
     <row r="69" spans="5:12">
@@ -5694,10 +5737,10 @@
         <v>0.14446666666666599</v>
       </c>
       <c r="K69" s="7">
-        <v>1.4200000000000001E-4</v>
+        <v>1.7899999999999999E-4</v>
       </c>
       <c r="L69" s="13">
-        <v>8.2799999999999996E-4</v>
+        <v>6.1190000000000003E-3</v>
       </c>
     </row>
     <row r="70" spans="5:12">
@@ -5720,10 +5763,10 @@
         <v>0.2717</v>
       </c>
       <c r="K70" s="7">
-        <v>2.42E-4</v>
+        <v>2.1900000000000001E-4</v>
       </c>
       <c r="L70" s="13">
-        <v>1.2329999999999999E-3</v>
+        <v>8.8000000000000005E-3</v>
       </c>
     </row>
     <row r="71" spans="5:12">
@@ -5746,10 +5789,10 @@
         <v>0.4541</v>
       </c>
       <c r="K71" s="7">
-        <v>3.0699999999999998E-4</v>
+        <v>2.5900000000000001E-4</v>
       </c>
       <c r="L71" s="13">
-        <v>1.7600000000000001E-3</v>
+        <v>1.157E-2</v>
       </c>
     </row>
     <row r="72" spans="5:12">
@@ -5772,10 +5815,10 @@
         <v>0.71935000000000004</v>
       </c>
       <c r="K72" s="7">
-        <v>4.17E-4</v>
+        <v>2.7999999999999998E-4</v>
       </c>
       <c r="L72" s="13">
-        <v>2.398E-3</v>
+        <v>1.4069999999999999E-2</v>
       </c>
     </row>
     <row r="73" spans="5:12">
@@ -5798,10 +5841,10 @@
         <v>1.1429</v>
       </c>
       <c r="K73" s="7">
-        <v>5.8399999999999999E-4</v>
+        <v>3.6900000000000002E-4</v>
       </c>
       <c r="L73" s="13">
-        <v>3.0469999999999998E-3</v>
+        <v>2.0889999999999999E-2</v>
       </c>
     </row>
     <row r="74" spans="5:12">
@@ -5824,10 +5867,10 @@
         <v>1.6839</v>
       </c>
       <c r="K74" s="7">
-        <v>8.3100000000000003E-4</v>
+        <v>5.1900000000000004E-4</v>
       </c>
       <c r="L74" s="13">
-        <v>4.1809999999999998E-3</v>
+        <v>2.7130000000000001E-2</v>
       </c>
     </row>
     <row r="75" spans="5:12">
@@ -5850,10 +5893,10 @@
         <v>2.4980000000000002</v>
       </c>
       <c r="K75" s="7">
-        <v>1.0709999999999999E-3</v>
+        <v>7.7899999999999996E-4</v>
       </c>
       <c r="L75" s="13">
-        <v>5.9280000000000001E-3</v>
+        <v>3.5400000000000001E-2</v>
       </c>
     </row>
     <row r="76" spans="5:12">
@@ -5876,10 +5919,10 @@
         <v>3.7126666666666601</v>
       </c>
       <c r="K76" s="7">
-        <v>1.2949999999999999E-3</v>
+        <v>1.0189999999999999E-3</v>
       </c>
       <c r="L76" s="13">
-        <v>9.1579999999999995E-3</v>
+        <v>4.9849999999999998E-2</v>
       </c>
     </row>
     <row r="77" spans="5:12">
@@ -5902,10 +5945,10 @@
         <v>4.9865000000000004</v>
       </c>
       <c r="K77" s="7">
-        <v>1.5900000000000001E-3</v>
+        <v>1.16E-3</v>
       </c>
       <c r="L77" s="13">
-        <v>1.273E-2</v>
+        <v>6.1679999999999999E-2</v>
       </c>
     </row>
     <row r="78" spans="5:12">
@@ -5928,10 +5971,10 @@
         <v>6.8185000000000002</v>
       </c>
       <c r="K78" s="7">
-        <v>1.882E-3</v>
+        <v>1.4189999999999999E-3</v>
       </c>
       <c r="L78" s="13">
-        <v>1.8724999999999999E-2</v>
+        <v>7.5380000000000003E-2</v>
       </c>
     </row>
     <row r="79" spans="5:12">
@@ -5954,10 +5997,10 @@
         <v>9.1835000000000004</v>
       </c>
       <c r="K79" s="7">
-        <v>2.4220000000000001E-3</v>
+        <v>1.7390000000000001E-3</v>
       </c>
       <c r="L79" s="13">
-        <v>2.7199999999999998E-2</v>
+        <v>9.3100000000000002E-2</v>
       </c>
     </row>
     <row r="80" spans="5:12">
@@ -5980,10 +6023,10 @@
         <v>12.628</v>
       </c>
       <c r="K80" s="7">
-        <v>2.7520000000000001E-3</v>
+        <v>1.8500000000000001E-3</v>
       </c>
       <c r="L80" s="13">
-        <v>3.5430000000000003E-2</v>
+        <v>0.116274</v>
       </c>
     </row>
     <row r="81" spans="5:12">
@@ -6006,10 +6049,10 @@
         <v>17.083500000000001</v>
       </c>
       <c r="K81" s="7">
-        <v>3.176E-3</v>
+        <v>2.1900000000000001E-3</v>
       </c>
       <c r="L81" s="13">
-        <v>4.4810000000000003E-2</v>
+        <v>0.13095000000000001</v>
       </c>
     </row>
     <row r="82" spans="5:12">
@@ -6032,10 +6075,10 @@
         <v>21.6525</v>
       </c>
       <c r="K82" s="7">
-        <v>3.692E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="L82" s="13">
-        <v>5.8700000000000002E-2</v>
+        <v>0.15928</v>
       </c>
     </row>
     <row r="83" spans="5:12">
@@ -6058,10 +6101,10 @@
         <v>29.923999999999999</v>
       </c>
       <c r="K83" s="7">
-        <v>4.2249999999999996E-3</v>
+        <v>2.7399999999999998E-3</v>
       </c>
       <c r="L83" s="13">
-        <v>7.3520000000000002E-2</v>
+        <v>0.18890000000000001</v>
       </c>
     </row>
     <row r="84" spans="5:12">
@@ -6084,10 +6127,10 @@
         <v>35.185000000000002</v>
       </c>
       <c r="K84" s="7">
-        <v>4.6100000000000004E-3</v>
+        <v>3.15E-3</v>
       </c>
       <c r="L84" s="13">
-        <v>8.8429999999999995E-2</v>
+        <v>0.21460000000000001</v>
       </c>
     </row>
     <row r="85" spans="5:12">
@@ -6110,10 +6153,10 @@
         <v>46.423499999999997</v>
       </c>
       <c r="K85" s="7">
-        <v>5.1900000000000002E-3</v>
+        <v>3.4499999999999999E-3</v>
       </c>
       <c r="L85" s="13">
-        <v>0.11020000000000001</v>
+        <v>0.25740000000000002</v>
       </c>
     </row>
     <row r="86" spans="5:12">
@@ -6136,10 +6179,46 @@
         <v>57.901499999999999</v>
       </c>
       <c r="K86" s="7">
-        <v>5.7800000000000004E-3</v>
+        <v>3.8500000000000001E-3</v>
       </c>
       <c r="L86" s="13">
-        <v>0.12706999999999999</v>
+        <v>0.26429999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="5:12">
+      <c r="F87">
+        <v>65160</v>
+      </c>
+      <c r="K87">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="L87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="5:12">
+      <c r="F88" s="5">
+        <v>80000</v>
+      </c>
+      <c r="K88" t="s">
+        <v>20</v>
+      </c>
+      <c r="L88" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="5:12">
+      <c r="F89">
+        <v>104424</v>
+      </c>
+      <c r="G89" t="s">
+        <v>22</v>
+      </c>
+      <c r="K89" t="s">
+        <v>24</v>
+      </c>
+      <c r="L89" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="128" ht="15.75" thickBot="1"/>
@@ -6217,16 +6296,16 @@
     </row>
     <row r="140" spans="4:10" ht="15.75" thickBot="1">
       <c r="F140" t="s">
+        <v>14</v>
+      </c>
+      <c r="G140" t="s">
         <v>15</v>
       </c>
-      <c r="G140" t="s">
+      <c r="H140" t="s">
         <v>16</v>
       </c>
-      <c r="H140" t="s">
+      <c r="I140" t="s">
         <v>17</v>
-      </c>
-      <c r="I140" t="s">
-        <v>14</v>
       </c>
       <c r="J140" t="s">
         <v>18</v>
@@ -6271,13 +6350,13 @@
         <f>1.95973706966682-0.0053390356114687*D142+0.0000027282285294*D142^2</f>
         <v>1.5305084588068953</v>
       </c>
-      <c r="I142" s="23">
-        <f>-0.000609+0.00000108*D142</f>
-        <v>-5.1827999999999998E-4</v>
-      </c>
-      <c r="J142" s="23">
-        <f>-0.0178824102691862+0.0000207193142874*D142</f>
-        <v>-1.61419878690446E-2</v>
+      <c r="I142" s="22">
+        <f>-0.0003470911688645 +0.0000007125249395*D142</f>
+        <v>-2.8723907394650002E-4</v>
+      </c>
+      <c r="J142">
+        <f>-0.0316993039054592+0.0000491746627289*D142</f>
+        <v>-2.7568632236231599E-2</v>
       </c>
     </row>
     <row r="143" spans="4:10">
@@ -6285,24 +6364,24 @@
         <v>144</v>
       </c>
       <c r="F143" s="8">
-        <f t="shared" ref="F143:F165" si="0">0.238782369320571 -0.0008012150098502 *D143+0.0000003535496443 *D143^2+0.0000000002725663 * D143^3</f>
+        <f t="shared" ref="F143:F166" si="0">0.238782369320571 -0.0008012150098502 *D143+0.0000003535496443 *D143^2+0.0000000002725663 * D143^3</f>
         <v>0.13155249193708621</v>
       </c>
       <c r="G143" s="5">
-        <f t="shared" ref="G143:G165" si="1">0.236700627690309-0.0005740326308383*D143+0.0000002405910959*D143^2</f>
+        <f t="shared" ref="G143:G166" si="1">0.236700627690309-0.0005740326308383*D143+0.0000002405910959*D143^2</f>
         <v>0.15902882581417618</v>
       </c>
       <c r="H143" s="21">
-        <f t="shared" ref="H143:H165" si="2">1.95973706966682-0.0053390356114687*D143+0.0000027282285294*D143^2</f>
+        <f t="shared" ref="H143:H166" si="2">1.95973706966682-0.0053390356114687*D143+0.0000027282285294*D143^2</f>
         <v>1.2474884884009654</v>
       </c>
-      <c r="I143" s="23">
-        <f t="shared" ref="I143:I165" si="3">-0.000609+0.00000108*D143</f>
-        <v>-4.5347999999999992E-4</v>
-      </c>
-      <c r="J143" s="23">
-        <f t="shared" ref="J143:J165" si="4">-0.0178824102691862+0.0000207193142874*D143</f>
-        <v>-1.4898829011800599E-2</v>
+      <c r="I143" s="22">
+        <f t="shared" ref="I143:I166" si="3">-0.0003470911688645 +0.0000007125249395*D143</f>
+        <v>-2.4448757757650002E-4</v>
+      </c>
+      <c r="J143">
+        <f t="shared" ref="J143:J166" si="4">-0.0316993039054592+0.0000491746627289*D143</f>
+        <v>-2.4618152472497601E-2</v>
       </c>
     </row>
     <row r="144" spans="4:10">
@@ -6321,13 +6400,13 @@
         <f t="shared" si="2"/>
         <v>0.91719549596666594</v>
       </c>
-      <c r="I144" s="23">
+      <c r="I144" s="22">
         <f t="shared" si="3"/>
-        <v>-3.7139999999999992E-4</v>
-      </c>
-      <c r="J144" s="23">
+        <v>-1.9033568217450002E-4</v>
+      </c>
+      <c r="J144">
         <f t="shared" si="4"/>
-        <v>-1.33241611259582E-2</v>
+        <v>-2.0880878105101197E-2</v>
       </c>
     </row>
     <row r="145" spans="4:10">
@@ -6346,20 +6425,20 @@
         <f t="shared" si="2"/>
         <v>0.55953463685449911</v>
       </c>
-      <c r="I145" s="23">
+      <c r="I145" s="22">
         <f t="shared" si="3"/>
-        <v>-2.7203999999999992E-4</v>
-      </c>
-      <c r="J145" s="23">
+        <v>-1.2478338774050003E-4</v>
+      </c>
+      <c r="J145">
         <f t="shared" si="4"/>
-        <v>-1.14179842115174E-2</v>
+        <v>-1.6356809134042399E-2</v>
       </c>
     </row>
     <row r="146" spans="4:10">
       <c r="D146" s="5">
         <v>420</v>
       </c>
-      <c r="F146" s="23">
+      <c r="F146" s="22">
         <f t="shared" si="0"/>
         <v>-1.5167885527592993E-2</v>
       </c>
@@ -6371,88 +6450,88 @@
         <f t="shared" si="2"/>
         <v>0.19860162543612575</v>
       </c>
-      <c r="I146" s="23">
+      <c r="I146" s="22">
         <f t="shared" si="3"/>
-        <v>-1.5539999999999993E-4</v>
-      </c>
-      <c r="J146" s="23">
+        <v>-4.783069427450004E-5</v>
+      </c>
+      <c r="J146">
         <f t="shared" si="4"/>
-        <v>-9.1802982684781997E-3</v>
+        <v>-1.1045945559321198E-2</v>
       </c>
     </row>
     <row r="147" spans="4:10">
       <c r="D147" s="5">
         <v>544</v>
       </c>
-      <c r="F147" s="23">
+      <c r="F147" s="22">
         <f t="shared" si="0"/>
         <v>-4.8570302279473773E-2</v>
       </c>
-      <c r="G147" s="23">
+      <c r="G147" s="22">
         <f t="shared" si="1"/>
         <v>-4.373556929463826E-3</v>
       </c>
-      <c r="H147" s="23">
+      <c r="H147" s="22">
         <f t="shared" si="2"/>
         <v>-0.13731726489563456</v>
       </c>
       <c r="I147" s="23">
         <f t="shared" si="3"/>
-        <v>-2.1479999999999937E-5</v>
-      </c>
-      <c r="J147" s="23">
+        <v>4.0522398223499941E-5</v>
+      </c>
+      <c r="J147">
         <f t="shared" si="4"/>
-        <v>-6.6111032968405991E-3</v>
+        <v>-4.9482873809376E-3</v>
       </c>
     </row>
     <row r="148" spans="4:10">
       <c r="D148" s="5">
         <v>684</v>
       </c>
-      <c r="F148" s="23">
+      <c r="F148" s="22">
         <f t="shared" si="0"/>
         <v>-5.6613478298029762E-2</v>
       </c>
-      <c r="G148" s="23">
+      <c r="G148" s="22">
         <f t="shared" si="1"/>
         <v>-4.3375704039697829E-2</v>
       </c>
-      <c r="H148" s="23">
+      <c r="H148" s="22">
         <f t="shared" si="2"/>
         <v>-0.41574520172680463</v>
       </c>
-      <c r="I148" s="5">
+      <c r="I148" s="23">
         <f t="shared" si="3"/>
-        <v>1.2972000000000005E-4</v>
-      </c>
-      <c r="J148" s="23">
+        <v>1.4027588975349997E-4</v>
+      </c>
+      <c r="J148">
         <f t="shared" si="4"/>
-        <v>-3.7103992966045999E-3</v>
+        <v>1.9361654011084001E-3</v>
       </c>
     </row>
     <row r="149" spans="4:10">
       <c r="D149" s="5">
         <v>840</v>
       </c>
-      <c r="F149" s="23">
+      <c r="F149" s="22">
         <f t="shared" si="0"/>
         <v>-2.3222473660317017E-2</v>
       </c>
-      <c r="G149" s="23">
+      <c r="G149" s="22">
         <f t="shared" si="1"/>
         <v>-7.5725704946823041E-2</v>
       </c>
-      <c r="H149" s="23">
+      <c r="H149" s="22">
         <f t="shared" si="2"/>
         <v>-0.60001479362224841</v>
       </c>
-      <c r="I149" s="5">
+      <c r="I149" s="23">
         <f t="shared" si="3"/>
-        <v>2.9820000000000009E-4</v>
-      </c>
-      <c r="J149" s="23">
-        <f>-0.0178824102691862+0.0000207193142874*D149</f>
-        <v>-4.7818626777020035E-4</v>
+        <v>2.5142978031549994E-4</v>
+      </c>
+      <c r="J149">
+        <f t="shared" si="4"/>
+        <v>9.6074127868168019E-3</v>
       </c>
     </row>
     <row r="150" spans="4:10">
@@ -6463,21 +6542,21 @@
         <f t="shared" si="0"/>
         <v>7.2535432700314262E-2</v>
       </c>
-      <c r="G150" s="23">
+      <c r="G150" s="22">
         <f t="shared" si="1"/>
         <v>-9.7820467398641059E-2</v>
       </c>
-      <c r="H150" s="23">
+      <c r="H150" s="22">
         <f t="shared" si="2"/>
         <v>-0.64926809012567066</v>
       </c>
-      <c r="I150" s="5">
+      <c r="I150" s="23">
         <f t="shared" si="3"/>
-        <v>4.8396000000000008E-4</v>
-      </c>
-      <c r="J150" s="22">
+        <v>3.7398406990949996E-4</v>
+      </c>
+      <c r="J150">
         <f t="shared" si="4"/>
-        <v>3.0855357896625996E-3</v>
+        <v>1.8065454776187602E-2</v>
       </c>
     </row>
     <row r="151" spans="4:10">
@@ -6488,21 +6567,21 @@
         <f t="shared" si="0"/>
         <v>0.257430411692331</v>
       </c>
-      <c r="G151" s="23">
+      <c r="G151" s="22">
         <f t="shared" si="1"/>
         <v>-0.105687351219651</v>
       </c>
-      <c r="H151" s="23">
+      <c r="H151" s="22">
         <f t="shared" si="2"/>
         <v>-0.51845658175962006</v>
       </c>
-      <c r="I151" s="5">
+      <c r="I151" s="23">
         <f t="shared" si="3"/>
-        <v>6.8700000000000011E-4</v>
-      </c>
-      <c r="J151" s="22">
+        <v>5.0793875853549992E-4</v>
+      </c>
+      <c r="J151">
         <f t="shared" si="4"/>
-        <v>6.9807668756937981E-3</v>
+        <v>2.73102913692208E-2</v>
       </c>
     </row>
     <row r="152" spans="4:10">
@@ -6513,21 +6592,21 @@
         <f t="shared" si="0"/>
         <v>0.56515023160496225</v>
       </c>
-      <c r="G152" s="23">
+      <c r="G152" s="22">
         <f t="shared" si="1"/>
         <v>-9.4984168311049888E-2</v>
       </c>
-      <c r="H152" s="23">
+      <c r="H152" s="22">
         <f t="shared" si="2"/>
         <v>-0.15834120002548424</v>
       </c>
-      <c r="I152" s="5">
+      <c r="I152" s="23">
         <f t="shared" si="3"/>
-        <v>9.0732000000000009E-4</v>
-      </c>
-      <c r="J152" s="22">
+        <v>6.5329384619349992E-4</v>
+      </c>
+      <c r="J152">
         <f t="shared" si="4"/>
-        <v>1.1207506990323399E-2</v>
+        <v>3.7341922565916404E-2</v>
       </c>
     </row>
     <row r="153" spans="4:10">
@@ -6538,7 +6617,7 @@
         <f t="shared" si="0"/>
         <v>1.0374808844879744</v>
       </c>
-      <c r="G153" s="23">
+      <c r="G153" s="22">
         <f t="shared" si="1"/>
         <v>-6.0999182650731898E-2</v>
       </c>
@@ -6546,13 +6625,13 @@
         <f t="shared" si="2"/>
         <v>0.48450768259650534</v>
       </c>
-      <c r="I153" s="5">
+      <c r="I153" s="23">
         <f t="shared" si="3"/>
-        <v>1.14492E-3</v>
-      </c>
-      <c r="J153" s="22">
+        <v>8.1004933288350003E-4</v>
+      </c>
+      <c r="J153">
         <f t="shared" si="4"/>
-        <v>1.5765756133551401E-2</v>
+        <v>4.8160348366274398E-2</v>
       </c>
     </row>
     <row r="154" spans="4:10">
@@ -6571,13 +6650,13 @@
         <f t="shared" si="2"/>
         <v>1.4677102526472776</v>
       </c>
-      <c r="I154" s="5">
+      <c r="I154" s="23">
         <f t="shared" si="3"/>
-        <v>1.3998000000000003E-3</v>
-      </c>
-      <c r="J154" s="22">
+        <v>9.7820521860550002E-4</v>
+      </c>
+      <c r="J154">
         <f t="shared" si="4"/>
-        <v>2.0655514305377796E-2</v>
+        <v>5.9765568770294798E-2</v>
       </c>
     </row>
     <row r="155" spans="4:10">
@@ -6596,13 +6675,13 @@
         <f t="shared" si="2"/>
         <v>2.8530772556889197</v>
       </c>
-      <c r="I155" s="5">
+      <c r="I155" s="23">
         <f t="shared" si="3"/>
-        <v>1.6719600000000003E-3</v>
-      </c>
-      <c r="J155" s="22">
+        <v>1.1577615033594999E-3</v>
+      </c>
+      <c r="J155">
         <f t="shared" si="4"/>
-        <v>2.5876781505802599E-2</v>
+        <v>7.2157583777977596E-2</v>
       </c>
     </row>
     <row r="156" spans="4:10">
@@ -6621,13 +6700,13 @@
         <f t="shared" si="2"/>
         <v>4.7066099963046746</v>
       </c>
-      <c r="I156" s="5">
+      <c r="I156" s="23">
         <f t="shared" si="3"/>
-        <v>1.9614000000000003E-3</v>
-      </c>
-      <c r="J156" s="22">
+        <v>1.3487181871454999E-3</v>
+      </c>
+      <c r="J156">
         <f t="shared" si="4"/>
-        <v>3.1429557734825794E-2</v>
+        <v>8.5336393389322807E-2</v>
       </c>
     </row>
     <row r="157" spans="4:10">
@@ -6646,13 +6725,13 @@
         <f t="shared" si="2"/>
         <v>7.0985003380989458</v>
       </c>
-      <c r="I157" s="5">
+      <c r="I157" s="23">
         <f t="shared" si="3"/>
-        <v>2.2681200000000002E-3</v>
-      </c>
-      <c r="J157" s="22">
+        <v>1.5510752699635E-3</v>
+      </c>
+      <c r="J157">
         <f t="shared" si="4"/>
-        <v>3.7313842992447402E-2</v>
+        <v>9.9301997604330394E-2</v>
       </c>
     </row>
     <row r="158" spans="4:10">
@@ -6671,13 +6750,13 @@
         <f t="shared" si="2"/>
         <v>10.103130703697296</v>
       </c>
-      <c r="I158" s="5">
+      <c r="I158" s="23">
         <f t="shared" si="3"/>
-        <v>2.5921199999999998E-3</v>
-      </c>
-      <c r="J158" s="22">
+        <v>1.7648327518134999E-3</v>
+      </c>
+      <c r="J158">
         <f t="shared" si="4"/>
-        <v>4.3529637278667391E-2</v>
+        <v>0.11405439642300041</v>
       </c>
     </row>
     <row r="159" spans="4:10">
@@ -6696,13 +6775,13 @@
         <f t="shared" si="2"/>
         <v>13.799074074746445</v>
       </c>
-      <c r="I159" s="5">
+      <c r="I159" s="23">
         <f t="shared" si="3"/>
-        <v>2.9334000000000001E-3</v>
-      </c>
-      <c r="J159" s="22">
+        <v>1.9899906326954998E-3</v>
+      </c>
+      <c r="J159">
         <f t="shared" si="4"/>
-        <v>5.0076940593485789E-2</v>
+        <v>0.12959358984533281</v>
       </c>
     </row>
     <row r="160" spans="4:10">
@@ -6721,13 +6800,13 @@
         <f t="shared" si="2"/>
         <v>18.269093991914264</v>
       </c>
-      <c r="I160" s="5">
+      <c r="I160" s="23">
         <f t="shared" si="3"/>
-        <v>3.29196E-3</v>
-      </c>
-      <c r="J160" s="22">
+        <v>2.2265489126094998E-3</v>
+      </c>
+      <c r="J160">
         <f t="shared" si="4"/>
-        <v>5.6955752936902596E-2</v>
+        <v>0.14591957787132759</v>
       </c>
     </row>
     <row r="161" spans="4:10">
@@ -6746,13 +6825,13 @@
         <f t="shared" si="2"/>
         <v>23.600144554889802</v>
       </c>
-      <c r="I161" s="5">
+      <c r="I161" s="23">
         <f t="shared" si="3"/>
-        <v>3.6677999999999997E-3</v>
-      </c>
-      <c r="J161" s="22">
+        <v>2.4745075915554998E-3</v>
+      </c>
+      <c r="J161">
         <f t="shared" si="4"/>
-        <v>6.4166074308917798E-2</v>
+        <v>0.1630323605009848</v>
       </c>
     </row>
     <row r="162" spans="4:10">
@@ -6771,13 +6850,13 @@
         <f t="shared" si="2"/>
         <v>29.883370422383251</v>
       </c>
-      <c r="I162" s="5">
+      <c r="I162" s="23">
         <f t="shared" si="3"/>
-        <v>4.06092E-3</v>
-      </c>
-      <c r="J162" s="22">
+        <v>2.7338666695335E-3</v>
+      </c>
+      <c r="J162">
         <f t="shared" si="4"/>
-        <v>7.1707904709531395E-2</v>
+        <v>0.18093193773430441</v>
       </c>
     </row>
     <row r="163" spans="4:10">
@@ -6796,13 +6875,13 @@
         <f t="shared" si="2"/>
         <v>37.214106812125962</v>
       </c>
-      <c r="I163" s="5">
+      <c r="I163" s="23">
         <f t="shared" si="3"/>
-        <v>4.47132E-3</v>
-      </c>
-      <c r="J163" s="22">
+        <v>3.0046261465434998E-3</v>
+      </c>
+      <c r="J163">
         <f t="shared" si="4"/>
-        <v>7.9581244138743387E-2</v>
+        <v>0.1996183095712864</v>
       </c>
     </row>
     <row r="164" spans="4:10">
@@ -6821,13 +6900,13 @@
         <f t="shared" si="2"/>
         <v>45.691879500870442</v>
       </c>
-      <c r="I164" s="5">
+      <c r="I164" s="23">
         <f t="shared" si="3"/>
-        <v>4.8989999999999997E-3</v>
-      </c>
-      <c r="J164" s="22">
+        <v>3.2867860225854998E-3</v>
+      </c>
+      <c r="J164">
         <f t="shared" si="4"/>
-        <v>8.7786092596553789E-2</v>
+        <v>0.21909147601193077</v>
       </c>
     </row>
     <row r="165" spans="4:10">
@@ -6846,13 +6925,43 @@
         <f t="shared" si="2"/>
         <v>55.420404824390374</v>
       </c>
-      <c r="I165" s="5">
+      <c r="I165" s="23">
         <f t="shared" si="3"/>
-        <v>5.34396E-3</v>
-      </c>
-      <c r="J165" s="22">
+        <v>3.5803462976594998E-3</v>
+      </c>
+      <c r="J165">
         <f t="shared" si="4"/>
-        <v>9.6322450082962585E-2</v>
+        <v>0.2393514370562376</v>
+      </c>
+    </row>
+    <row r="166" spans="4:10">
+      <c r="D166" s="5">
+        <v>65160</v>
+      </c>
+      <c r="F166" s="8">
+        <f t="shared" si="0"/>
+        <v>76856.788104268475</v>
+      </c>
+      <c r="G166" s="5">
+        <f t="shared" si="1"/>
+        <v>984.34056850654179</v>
+      </c>
+      <c r="H166" s="21">
+        <f t="shared" si="2"/>
+        <v>11237.650709403239</v>
+      </c>
+      <c r="I166" s="23">
+        <f t="shared" si="3"/>
+        <v>4.60810338889555E-2</v>
+      </c>
+      <c r="J166">
+        <f t="shared" si="4"/>
+        <v>3.1725217195096649</v>
+      </c>
+    </row>
+    <row r="167" spans="4:10">
+      <c r="D167">
+        <v>104424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>